<commit_message>
Labeled half of the data
</commit_message>
<xml_diff>
--- a/venv/assets/commentsArabic.xlsx
+++ b/venv/assets/commentsArabic.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ask-Banky-Classifier\venv\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{65340071-6C1B-458B-B25D-BA39FA1B36C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A714383-FC5C-401C-A349-C22976A83F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="1068" yWindow="3132" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commentsArabic" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="727">
   <si>
     <t>comment_id</t>
   </si>
@@ -2206,7 +2206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3040,11 +3040,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D817"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H238" sqref="H238"/>
+    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
+      <selection activeCell="F330" sqref="F330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6699,6 +6699,9 @@
       <c r="C261">
         <v>51</v>
       </c>
+      <c r="D261" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262">
@@ -6710,6 +6713,9 @@
       <c r="C262">
         <v>52</v>
       </c>
+      <c r="D262" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263">
@@ -6721,6 +6727,9 @@
       <c r="C263">
         <v>52</v>
       </c>
+      <c r="D263" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264">
@@ -6732,6 +6741,9 @@
       <c r="C264">
         <v>53</v>
       </c>
+      <c r="D264" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265">
@@ -6743,6 +6755,9 @@
       <c r="C265">
         <v>53</v>
       </c>
+      <c r="D265" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266">
@@ -6754,6 +6769,9 @@
       <c r="C266">
         <v>53</v>
       </c>
+      <c r="D266" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267">
@@ -6765,6 +6783,9 @@
       <c r="C267">
         <v>53</v>
       </c>
+      <c r="D267" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268">
@@ -6776,6 +6797,9 @@
       <c r="C268">
         <v>53</v>
       </c>
+      <c r="D268" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269">
@@ -6787,6 +6811,9 @@
       <c r="C269">
         <v>53</v>
       </c>
+      <c r="D269" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
@@ -6798,6 +6825,9 @@
       <c r="C270">
         <v>53</v>
       </c>
+      <c r="D270" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
@@ -6809,6 +6839,9 @@
       <c r="C271">
         <v>53</v>
       </c>
+      <c r="D271" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
@@ -6820,8 +6853,11 @@
       <c r="C272">
         <v>54</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D272" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
@@ -6831,8 +6867,11 @@
       <c r="C273">
         <v>55</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D273" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
@@ -6842,8 +6881,11 @@
       <c r="C274">
         <v>55</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D274" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
@@ -6853,8 +6895,11 @@
       <c r="C275">
         <v>58</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D275" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
@@ -6864,8 +6909,11 @@
       <c r="C276">
         <v>58</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D276" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
@@ -6875,8 +6923,11 @@
       <c r="C277">
         <v>59</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D277" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
@@ -6886,8 +6937,11 @@
       <c r="C278">
         <v>59</v>
       </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D278" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
@@ -6897,8 +6951,11 @@
       <c r="C279">
         <v>60</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D279" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
@@ -6908,8 +6965,11 @@
       <c r="C280">
         <v>60</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D280" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
@@ -6919,8 +6979,11 @@
       <c r="C281">
         <v>61</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D281" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
@@ -6930,8 +6993,11 @@
       <c r="C282">
         <v>61</v>
       </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D282" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
@@ -6941,8 +7007,11 @@
       <c r="C283">
         <v>62</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D283" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
@@ -6952,8 +7021,11 @@
       <c r="C284">
         <v>62</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D284" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
@@ -6963,8 +7035,11 @@
       <c r="C285">
         <v>63</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D285" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
@@ -6974,8 +7049,11 @@
       <c r="C286">
         <v>64</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D286" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
@@ -6985,8 +7063,11 @@
       <c r="C287">
         <v>65</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D287" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
@@ -6996,8 +7077,11 @@
       <c r="C288">
         <v>65</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D288" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
@@ -7007,8 +7091,11 @@
       <c r="C289">
         <v>67</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D289" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
@@ -7018,8 +7105,11 @@
       <c r="C290">
         <v>67</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D290" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
@@ -7029,8 +7119,11 @@
       <c r="C291">
         <v>68</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D291" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
@@ -7040,8 +7133,11 @@
       <c r="C292">
         <v>69</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D292" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
@@ -7051,8 +7147,11 @@
       <c r="C293">
         <v>69</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D293" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
@@ -7062,8 +7161,11 @@
       <c r="C294">
         <v>70</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D294" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
@@ -7073,8 +7175,11 @@
       <c r="C295">
         <v>70</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D295" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
@@ -7084,8 +7189,11 @@
       <c r="C296">
         <v>71</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D296" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
@@ -7095,8 +7203,11 @@
       <c r="C297">
         <v>72</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D297" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
@@ -7106,8 +7217,11 @@
       <c r="C298">
         <v>72</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D298" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
@@ -7117,8 +7231,11 @@
       <c r="C299">
         <v>73</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D299" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
@@ -7128,8 +7245,11 @@
       <c r="C300">
         <v>74</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D300" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
@@ -7139,8 +7259,11 @@
       <c r="C301">
         <v>75</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D301" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
@@ -7150,8 +7273,11 @@
       <c r="C302">
         <v>76</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D302" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
@@ -7161,8 +7287,11 @@
       <c r="C303">
         <v>77</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D303" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
@@ -7172,8 +7301,11 @@
       <c r="C304">
         <v>78</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D304" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
@@ -7183,8 +7315,11 @@
       <c r="C305">
         <v>79</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D305" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
@@ -7194,8 +7329,11 @@
       <c r="C306">
         <v>80</v>
       </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D306" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
@@ -7205,8 +7343,11 @@
       <c r="C307">
         <v>80</v>
       </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D307" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
@@ -7216,8 +7357,11 @@
       <c r="C308">
         <v>81</v>
       </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D308" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
@@ -7227,8 +7371,11 @@
       <c r="C309">
         <v>83</v>
       </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D309" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
@@ -7238,8 +7385,11 @@
       <c r="C310">
         <v>83</v>
       </c>
-    </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D310" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
@@ -7249,8 +7399,11 @@
       <c r="C311">
         <v>85</v>
       </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D311" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
@@ -7260,8 +7413,11 @@
       <c r="C312">
         <v>86</v>
       </c>
-    </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D312" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
@@ -7271,8 +7427,11 @@
       <c r="C313">
         <v>86</v>
       </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D313" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
@@ -7282,8 +7441,11 @@
       <c r="C314">
         <v>87</v>
       </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D314" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
@@ -7293,8 +7455,11 @@
       <c r="C315">
         <v>91</v>
       </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D315" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
@@ -7304,8 +7469,11 @@
       <c r="C316">
         <v>91</v>
       </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D316" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
@@ -7315,8 +7483,11 @@
       <c r="C317">
         <v>94</v>
       </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D317" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
@@ -7326,8 +7497,11 @@
       <c r="C318">
         <v>94</v>
       </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D318" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
@@ -7337,8 +7511,11 @@
       <c r="C319">
         <v>95</v>
       </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D319" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
@@ -7348,8 +7525,11 @@
       <c r="C320">
         <v>96</v>
       </c>
-    </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D320" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>320</v>
       </c>
@@ -7359,8 +7539,11 @@
       <c r="C321">
         <v>96</v>
       </c>
-    </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D321" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>321</v>
       </c>
@@ -7370,8 +7553,11 @@
       <c r="C322">
         <v>96</v>
       </c>
-    </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D322" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>322</v>
       </c>
@@ -7381,8 +7567,11 @@
       <c r="C323">
         <v>97</v>
       </c>
-    </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D323" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>323</v>
       </c>
@@ -7392,8 +7581,11 @@
       <c r="C324">
         <v>97</v>
       </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D324" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>324</v>
       </c>
@@ -7403,8 +7595,11 @@
       <c r="C325">
         <v>97</v>
       </c>
-    </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D325" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>325</v>
       </c>
@@ -7414,8 +7609,11 @@
       <c r="C326">
         <v>97</v>
       </c>
-    </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D326" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>326</v>
       </c>
@@ -7425,8 +7623,11 @@
       <c r="C327">
         <v>98</v>
       </c>
-    </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D327" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>327</v>
       </c>
@@ -7436,8 +7637,11 @@
       <c r="C328">
         <v>99</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D328" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>328</v>
       </c>
@@ -7447,8 +7651,11 @@
       <c r="C329">
         <v>99</v>
       </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D329" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>329</v>
       </c>
@@ -7458,8 +7665,11 @@
       <c r="C330">
         <v>100</v>
       </c>
-    </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D330" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>330</v>
       </c>
@@ -7470,7 +7680,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>331</v>
       </c>
@@ -7481,7 +7691,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>332</v>
       </c>
@@ -7492,7 +7702,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>333</v>
       </c>
@@ -7503,7 +7713,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>334</v>
       </c>
@@ -7514,7 +7724,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>335</v>
       </c>

</xml_diff>

<commit_message>
Labelled 75% of the data
</commit_message>
<xml_diff>
--- a/venv/assets/commentsArabic.xlsx
+++ b/venv/assets/commentsArabic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ask-Banky-Classifier\venv\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A714383-FC5C-401C-A349-C22976A83F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17CFC5F-C19A-4AA9-BE50-35A08E6342D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="3132" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="728">
   <si>
     <t>comment_id</t>
   </si>
@@ -2201,6 +2201,9 @@
   </si>
   <si>
     <t>تحويلات</t>
+  </si>
+  <si>
+    <t>معلومة</t>
   </si>
 </sst>
 </file>
@@ -3043,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D817"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A320" workbookViewId="0">
-      <selection activeCell="F330" sqref="F330"/>
+    <sheetView tabSelected="1" topLeftCell="A425" workbookViewId="0">
+      <selection activeCell="H433" sqref="H433"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7679,6 +7682,9 @@
       <c r="C331">
         <v>101</v>
       </c>
+      <c r="D331" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332">
@@ -7690,6 +7696,9 @@
       <c r="C332">
         <v>103</v>
       </c>
+      <c r="D332" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333">
@@ -7701,6 +7710,9 @@
       <c r="C333">
         <v>104</v>
       </c>
+      <c r="D333" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334">
@@ -7712,6 +7724,9 @@
       <c r="C334">
         <v>104</v>
       </c>
+      <c r="D334" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335">
@@ -7723,6 +7738,9 @@
       <c r="C335">
         <v>105</v>
       </c>
+      <c r="D335" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336">
@@ -7734,8 +7752,11 @@
       <c r="C336">
         <v>106</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D336" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>336</v>
       </c>
@@ -7745,8 +7766,11 @@
       <c r="C337">
         <v>106</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D337" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>337</v>
       </c>
@@ -7756,8 +7780,11 @@
       <c r="C338">
         <v>107</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D338" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>338</v>
       </c>
@@ -7767,8 +7794,11 @@
       <c r="C339">
         <v>107</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D339" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>339</v>
       </c>
@@ -7778,8 +7808,11 @@
       <c r="C340">
         <v>108</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D340" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>340</v>
       </c>
@@ -7789,8 +7822,11 @@
       <c r="C341">
         <v>109</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D341" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>341</v>
       </c>
@@ -7800,8 +7836,11 @@
       <c r="C342">
         <v>109</v>
       </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D342" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>342</v>
       </c>
@@ -7811,8 +7850,11 @@
       <c r="C343">
         <v>109</v>
       </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D343" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>343</v>
       </c>
@@ -7822,8 +7864,11 @@
       <c r="C344">
         <v>109</v>
       </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D344" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>344</v>
       </c>
@@ -7833,8 +7878,11 @@
       <c r="C345">
         <v>112</v>
       </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D345" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>345</v>
       </c>
@@ -7844,8 +7892,11 @@
       <c r="C346">
         <v>113</v>
       </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D346" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>346</v>
       </c>
@@ -7855,8 +7906,11 @@
       <c r="C347">
         <v>114</v>
       </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D347" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>347</v>
       </c>
@@ -7866,8 +7920,11 @@
       <c r="C348">
         <v>114</v>
       </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D348" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>348</v>
       </c>
@@ -7877,8 +7934,11 @@
       <c r="C349">
         <v>115</v>
       </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D349" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>349</v>
       </c>
@@ -7888,8 +7948,11 @@
       <c r="C350">
         <v>116</v>
       </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D350" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>350</v>
       </c>
@@ -7899,8 +7962,11 @@
       <c r="C351">
         <v>118</v>
       </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D351" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>351</v>
       </c>
@@ -7910,8 +7976,11 @@
       <c r="C352">
         <v>118</v>
       </c>
-    </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D352" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>352</v>
       </c>
@@ -7921,8 +7990,11 @@
       <c r="C353">
         <v>118</v>
       </c>
-    </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D353" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>353</v>
       </c>
@@ -7932,8 +8004,11 @@
       <c r="C354">
         <v>119</v>
       </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D354" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>354</v>
       </c>
@@ -7943,8 +8018,11 @@
       <c r="C355">
         <v>120</v>
       </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D355" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>355</v>
       </c>
@@ -7954,8 +8032,11 @@
       <c r="C356">
         <v>120</v>
       </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D356" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>356</v>
       </c>
@@ -7965,8 +8046,11 @@
       <c r="C357">
         <v>120</v>
       </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D357" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>357</v>
       </c>
@@ -7976,8 +8060,11 @@
       <c r="C358">
         <v>120</v>
       </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D358" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>358</v>
       </c>
@@ -7987,8 +8074,11 @@
       <c r="C359">
         <v>120</v>
       </c>
-    </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D359" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>359</v>
       </c>
@@ -7998,8 +8088,11 @@
       <c r="C360">
         <v>120</v>
       </c>
-    </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D360" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>360</v>
       </c>
@@ -8009,8 +8102,11 @@
       <c r="C361">
         <v>120</v>
       </c>
-    </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D361" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>361</v>
       </c>
@@ -8020,8 +8116,11 @@
       <c r="C362">
         <v>121</v>
       </c>
-    </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D362" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>362</v>
       </c>
@@ -8031,8 +8130,11 @@
       <c r="C363">
         <v>124</v>
       </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D363" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>363</v>
       </c>
@@ -8042,8 +8144,11 @@
       <c r="C364">
         <v>125</v>
       </c>
-    </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D364" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>364</v>
       </c>
@@ -8053,8 +8158,11 @@
       <c r="C365">
         <v>125</v>
       </c>
-    </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D365" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>365</v>
       </c>
@@ -8064,8 +8172,11 @@
       <c r="C366">
         <v>125</v>
       </c>
-    </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D366" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>366</v>
       </c>
@@ -8075,8 +8186,11 @@
       <c r="C367">
         <v>125</v>
       </c>
-    </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D367" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>367</v>
       </c>
@@ -8086,8 +8200,11 @@
       <c r="C368">
         <v>125</v>
       </c>
-    </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D368" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>368</v>
       </c>
@@ -8097,8 +8214,11 @@
       <c r="C369">
         <v>126</v>
       </c>
-    </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D369" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>369</v>
       </c>
@@ -8108,8 +8228,11 @@
       <c r="C370">
         <v>126</v>
       </c>
-    </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D370" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>370</v>
       </c>
@@ -8119,8 +8242,11 @@
       <c r="C371">
         <v>126</v>
       </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D371" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>371</v>
       </c>
@@ -8130,8 +8256,11 @@
       <c r="C372">
         <v>126</v>
       </c>
-    </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D372" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>372</v>
       </c>
@@ -8141,8 +8270,11 @@
       <c r="C373">
         <v>126</v>
       </c>
-    </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D373" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>373</v>
       </c>
@@ -8152,8 +8284,11 @@
       <c r="C374">
         <v>127</v>
       </c>
-    </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D374" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>374</v>
       </c>
@@ -8163,8 +8298,11 @@
       <c r="C375">
         <v>127</v>
       </c>
-    </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D375" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>375</v>
       </c>
@@ -8174,8 +8312,11 @@
       <c r="C376">
         <v>128</v>
       </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D376" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>376</v>
       </c>
@@ -8185,8 +8326,11 @@
       <c r="C377">
         <v>128</v>
       </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D377" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>377</v>
       </c>
@@ -8196,8 +8340,11 @@
       <c r="C378">
         <v>128</v>
       </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D378" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>378</v>
       </c>
@@ -8207,8 +8354,11 @@
       <c r="C379">
         <v>128</v>
       </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D379" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>379</v>
       </c>
@@ -8218,8 +8368,11 @@
       <c r="C380">
         <v>128</v>
       </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D380" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>380</v>
       </c>
@@ -8229,8 +8382,11 @@
       <c r="C381">
         <v>128</v>
       </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D381" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>381</v>
       </c>
@@ -8240,8 +8396,11 @@
       <c r="C382">
         <v>129</v>
       </c>
-    </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D382" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>382</v>
       </c>
@@ -8251,8 +8410,11 @@
       <c r="C383">
         <v>129</v>
       </c>
-    </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D383" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>383</v>
       </c>
@@ -8262,8 +8424,11 @@
       <c r="C384">
         <v>129</v>
       </c>
-    </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D384" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>384</v>
       </c>
@@ -8273,8 +8438,11 @@
       <c r="C385">
         <v>129</v>
       </c>
-    </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D385" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>385</v>
       </c>
@@ -8284,8 +8452,11 @@
       <c r="C386">
         <v>129</v>
       </c>
-    </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D386" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>386</v>
       </c>
@@ -8295,8 +8466,11 @@
       <c r="C387">
         <v>129</v>
       </c>
-    </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D387" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>387</v>
       </c>
@@ -8306,8 +8480,11 @@
       <c r="C388">
         <v>129</v>
       </c>
-    </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D388" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>388</v>
       </c>
@@ -8317,8 +8494,11 @@
       <c r="C389">
         <v>130</v>
       </c>
-    </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D389" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>389</v>
       </c>
@@ -8328,8 +8508,11 @@
       <c r="C390">
         <v>131</v>
       </c>
-    </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D390" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>390</v>
       </c>
@@ -8339,8 +8522,11 @@
       <c r="C391">
         <v>131</v>
       </c>
-    </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D391" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>391</v>
       </c>
@@ -8350,8 +8536,11 @@
       <c r="C392">
         <v>133</v>
       </c>
-    </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D392" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>392</v>
       </c>
@@ -8361,8 +8550,11 @@
       <c r="C393">
         <v>133</v>
       </c>
-    </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D393" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>393</v>
       </c>
@@ -8372,8 +8564,11 @@
       <c r="C394">
         <v>134</v>
       </c>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D394" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>394</v>
       </c>
@@ -8383,8 +8578,11 @@
       <c r="C395">
         <v>135</v>
       </c>
-    </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D395" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>395</v>
       </c>
@@ -8394,8 +8592,11 @@
       <c r="C396">
         <v>136</v>
       </c>
-    </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D396" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>396</v>
       </c>
@@ -8405,8 +8606,11 @@
       <c r="C397">
         <v>137</v>
       </c>
-    </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D397" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>397</v>
       </c>
@@ -8416,8 +8620,11 @@
       <c r="C398">
         <v>137</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D398" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>398</v>
       </c>
@@ -8427,8 +8634,11 @@
       <c r="C399">
         <v>138</v>
       </c>
-    </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D399" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>399</v>
       </c>
@@ -8438,8 +8648,11 @@
       <c r="C400">
         <v>139</v>
       </c>
-    </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D400" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A401">
         <v>400</v>
       </c>
@@ -8449,8 +8662,11 @@
       <c r="C401">
         <v>139</v>
       </c>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D401" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A402">
         <v>401</v>
       </c>
@@ -8460,8 +8676,11 @@
       <c r="C402">
         <v>142</v>
       </c>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D402" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A403">
         <v>402</v>
       </c>
@@ -8471,8 +8690,11 @@
       <c r="C403">
         <v>142</v>
       </c>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D403" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A404">
         <v>403</v>
       </c>
@@ -8482,8 +8704,11 @@
       <c r="C404">
         <v>142</v>
       </c>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D404" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A405">
         <v>404</v>
       </c>
@@ -8493,8 +8718,11 @@
       <c r="C405">
         <v>142</v>
       </c>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D405" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>405</v>
       </c>
@@ -8504,8 +8732,11 @@
       <c r="C406">
         <v>143</v>
       </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D406" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>406</v>
       </c>
@@ -8515,8 +8746,11 @@
       <c r="C407">
         <v>143</v>
       </c>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D407" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>407</v>
       </c>
@@ -8526,8 +8760,11 @@
       <c r="C408">
         <v>143</v>
       </c>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D408" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>408</v>
       </c>
@@ -8537,8 +8774,11 @@
       <c r="C409">
         <v>143</v>
       </c>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D409" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>409</v>
       </c>
@@ -8548,8 +8788,11 @@
       <c r="C410">
         <v>143</v>
       </c>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D410" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>410</v>
       </c>
@@ -8559,8 +8802,11 @@
       <c r="C411">
         <v>144</v>
       </c>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D411" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>411</v>
       </c>
@@ -8570,8 +8816,11 @@
       <c r="C412">
         <v>144</v>
       </c>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D412" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>412</v>
       </c>
@@ -8581,8 +8830,11 @@
       <c r="C413">
         <v>144</v>
       </c>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D413" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A414">
         <v>413</v>
       </c>
@@ -8592,8 +8844,11 @@
       <c r="C414">
         <v>145</v>
       </c>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D414" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A415">
         <v>414</v>
       </c>
@@ -8603,8 +8858,11 @@
       <c r="C415">
         <v>145</v>
       </c>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D415" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A416">
         <v>415</v>
       </c>
@@ -8614,8 +8872,11 @@
       <c r="C416">
         <v>145</v>
       </c>
-    </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D416" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>416</v>
       </c>
@@ -8625,8 +8886,11 @@
       <c r="C417">
         <v>145</v>
       </c>
-    </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D417" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>417</v>
       </c>
@@ -8636,8 +8900,11 @@
       <c r="C418">
         <v>145</v>
       </c>
-    </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D418" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>418</v>
       </c>
@@ -8647,8 +8914,11 @@
       <c r="C419">
         <v>145</v>
       </c>
-    </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D419" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>419</v>
       </c>
@@ -8658,8 +8928,11 @@
       <c r="C420">
         <v>145</v>
       </c>
-    </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D420" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>420</v>
       </c>
@@ -8669,8 +8942,11 @@
       <c r="C421">
         <v>146</v>
       </c>
-    </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D421" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>421</v>
       </c>
@@ -8680,8 +8956,11 @@
       <c r="C422">
         <v>146</v>
       </c>
-    </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D422" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>422</v>
       </c>
@@ -8691,8 +8970,11 @@
       <c r="C423">
         <v>146</v>
       </c>
-    </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D423" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>423</v>
       </c>
@@ -8702,8 +8984,11 @@
       <c r="C424">
         <v>146</v>
       </c>
-    </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D424" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>424</v>
       </c>
@@ -8713,8 +8998,11 @@
       <c r="C425">
         <v>146</v>
       </c>
-    </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D425" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>425</v>
       </c>
@@ -8724,8 +9012,11 @@
       <c r="C426">
         <v>146</v>
       </c>
-    </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D426" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>426</v>
       </c>
@@ -8735,8 +9026,11 @@
       <c r="C427">
         <v>147</v>
       </c>
-    </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D427" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>427</v>
       </c>
@@ -8746,8 +9040,11 @@
       <c r="C428">
         <v>147</v>
       </c>
-    </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D428" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>428</v>
       </c>
@@ -8757,8 +9054,11 @@
       <c r="C429">
         <v>147</v>
       </c>
-    </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D429" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>429</v>
       </c>
@@ -8768,8 +9068,11 @@
       <c r="C430">
         <v>148</v>
       </c>
-    </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D430" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>430</v>
       </c>
@@ -8779,8 +9082,11 @@
       <c r="C431">
         <v>148</v>
       </c>
-    </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D431" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>431</v>
       </c>
@@ -8790,8 +9096,11 @@
       <c r="C432">
         <v>149</v>
       </c>
-    </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D432" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>432</v>
       </c>
@@ -8801,8 +9110,11 @@
       <c r="C433">
         <v>150</v>
       </c>
-    </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D433" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>433</v>
       </c>
@@ -8812,8 +9124,11 @@
       <c r="C434">
         <v>150</v>
       </c>
-    </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D434" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>434</v>
       </c>
@@ -8824,7 +9139,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>435</v>
       </c>
@@ -8835,7 +9150,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>436</v>
       </c>
@@ -8846,7 +9161,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>437</v>
       </c>
@@ -8857,7 +9172,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>438</v>
       </c>
@@ -8868,7 +9183,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>439</v>
       </c>
@@ -8879,7 +9194,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>440</v>
       </c>
@@ -8890,7 +9205,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>441</v>
       </c>
@@ -8901,7 +9216,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>442</v>
       </c>
@@ -8912,7 +9227,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>443</v>
       </c>
@@ -8923,7 +9238,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>444</v>
       </c>
@@ -8934,7 +9249,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>445</v>
       </c>
@@ -8945,7 +9260,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>446</v>
       </c>
@@ -8956,7 +9271,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>447</v>
       </c>

</xml_diff>

<commit_message>
Created csv files for each topic
</commit_message>
<xml_diff>
--- a/venv/assets/commentsArabic.xlsx
+++ b/venv/assets/commentsArabic.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ask-Banky-Classifier\venv\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAED168-15F9-4237-9D09-93C1FEDB03AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7546638-0ADC-4BB0-823B-2CA6CEB38852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commentsArabic" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">commentsArabic!$D$1:$D$817</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -3054,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D817"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C796" workbookViewId="0">
-      <selection activeCell="F815" sqref="F815"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14505,6 +14508,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D1:D817" xr:uid="{682C939C-B484-4137-893C-D65FC2DC5F35}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>